<commit_message>
add spawn times, verbose logs
</commit_message>
<xml_diff>
--- a/simulation/data/car_positions.xlsx
+++ b/simulation/data/car_positions.xlsx
@@ -436,12 +436,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>SE_CAR_A</t>
+          <t>SE_CAR_0</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>WS_CAR_B</t>
+          <t>WS_CAR_1</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor car creation and simulation code
</commit_message>
<xml_diff>
--- a/simulation/data/car_positions.xlsx
+++ b/simulation/data/car_positions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F104"/>
+  <dimension ref="A1:G110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,11 @@
           <t>WS_CAR_5</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>SE_CAR_6</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -496,6 +501,11 @@
           <t>(-50, 0)</t>
         </is>
       </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -528,6 +538,11 @@
           <t>(-50, 0)</t>
         </is>
       </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -537,7 +552,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>(-48.16, 0)</t>
+          <t>(-48.24, 0)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -558,6 +573,11 @@
       <c r="F4" t="inlineStr">
         <is>
           <t>(-50, 0)</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -569,7 +589,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>(-47.31999999999999, 0)</t>
+          <t>(-47.480000000000004, 0)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -590,6 +610,11 @@
       <c r="F5" t="inlineStr">
         <is>
           <t>(-50, 0)</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -601,7 +626,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>(-46.47999999999999, 0)</t>
+          <t>(-46.720000000000006, 0)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -622,6 +647,11 @@
       <c r="F6" t="inlineStr">
         <is>
           <t>(-50, 0)</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -633,7 +663,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>(-45.639999999999986, 0)</t>
+          <t>(-45.96000000000001, 0)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -654,6 +684,11 @@
       <c r="F7" t="inlineStr">
         <is>
           <t>(-50, 0)</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -665,7 +700,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>(-44.79999999999998, 0)</t>
+          <t>(-45.20000000000001, 0)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -686,6 +721,11 @@
       <c r="F8" t="inlineStr">
         <is>
           <t>(-50, 0)</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -697,7 +737,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>(-43.95999999999998, 0)</t>
+          <t>(-44.44000000000001, 0)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -718,6 +758,11 @@
       <c r="F9" t="inlineStr">
         <is>
           <t>(-50, 0)</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -729,7 +774,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>(-43.119999999999976, 0)</t>
+          <t>(-43.680000000000014, 0)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -750,6 +795,11 @@
       <c r="F10" t="inlineStr">
         <is>
           <t>(-50, 0)</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -761,7 +811,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>(-42.27999999999997, 0)</t>
+          <t>(-42.920000000000016, 0)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -782,6 +832,11 @@
       <c r="F11" t="inlineStr">
         <is>
           <t>(-50, 0)</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -793,7 +848,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>(-41.43999999999997, 0)</t>
+          <t>(-42.16000000000002, 0)</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -814,6 +869,11 @@
       <c r="F12" t="inlineStr">
         <is>
           <t>(-50, 0)</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -825,7 +885,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>(-40.599999999999966, 0)</t>
+          <t>(-41.40000000000002, 0)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -846,6 +906,11 @@
       <c r="F13" t="inlineStr">
         <is>
           <t>(-50, 0)</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -857,7 +922,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>(-39.75999999999996, 0)</t>
+          <t>(-40.64000000000002, 0)</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -878,6 +943,11 @@
       <c r="F14" t="inlineStr">
         <is>
           <t>(-50, 0)</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -889,7 +959,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>(-38.91999999999996, 0)</t>
+          <t>(-39.880000000000024, 0)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -910,6 +980,11 @@
       <c r="F15" t="inlineStr">
         <is>
           <t>(-50, 0)</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -921,7 +996,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>(-38.079999999999956, 0)</t>
+          <t>(-39.120000000000026, 0)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -942,6 +1017,11 @@
       <c r="F16" t="inlineStr">
         <is>
           <t>(-50, 0)</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -953,7 +1033,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>(-37.23999999999995, 0)</t>
+          <t>(-38.36000000000003, 0)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -974,6 +1054,11 @@
       <c r="F17" t="inlineStr">
         <is>
           <t>(-50, 0)</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -985,7 +1070,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>(-36.39999999999995, 0)</t>
+          <t>(-37.60000000000003, 0)</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1006,6 +1091,11 @@
       <c r="F18" t="inlineStr">
         <is>
           <t>(-50, 0)</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -1017,7 +1107,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>(-35.559999999999945, 0)</t>
+          <t>(-36.84000000000003, 0)</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1038,6 +1128,11 @@
       <c r="F19" t="inlineStr">
         <is>
           <t>(-50, 0)</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -1049,7 +1144,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>(-34.71999999999994, 0)</t>
+          <t>(-36.080000000000034, 0)</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1070,6 +1165,11 @@
       <c r="F20" t="inlineStr">
         <is>
           <t>(-50, 0)</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -1081,7 +1181,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>(-33.87999999999994, 0)</t>
+          <t>(-35.320000000000036, 0)</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1102,6 +1202,11 @@
       <c r="F21" t="inlineStr">
         <is>
           <t>(-50, 0)</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -1113,7 +1218,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>(-33.039999999999935, 0)</t>
+          <t>(-34.56000000000004, 0)</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1134,6 +1239,11 @@
       <c r="F22" t="inlineStr">
         <is>
           <t>(-50, 0)</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -1145,7 +1255,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>(-32.19999999999993, 0)</t>
+          <t>(-33.80000000000004, 0)</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1166,6 +1276,11 @@
       <c r="F23" t="inlineStr">
         <is>
           <t>(-50, 0)</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -1177,7 +1292,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>(-31.359999999999932, 0)</t>
+          <t>(-33.04000000000004, 0)</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1198,6 +1313,11 @@
       <c r="F24" t="inlineStr">
         <is>
           <t>(-50, 0)</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -1209,7 +1329,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>(-30.519999999999932, 0)</t>
+          <t>(-32.280000000000044, 0)</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1230,6 +1350,11 @@
       <c r="F25" t="inlineStr">
         <is>
           <t>(-50, 0)</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -1241,7 +1366,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>(-29.679999999999932, 0)</t>
+          <t>(-31.520000000000042, 0)</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1262,6 +1387,11 @@
       <c r="F26" t="inlineStr">
         <is>
           <t>(-50, 0)</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -1273,7 +1403,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>(-28.839999999999932, 0)</t>
+          <t>(-30.76000000000004, 0)</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1294,6 +1424,11 @@
       <c r="F27" t="inlineStr">
         <is>
           <t>(-50, 0)</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -1305,7 +1440,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>(-27.999999999999932, 0)</t>
+          <t>(-30.00000000000004, 0)</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1326,6 +1461,11 @@
       <c r="F28" t="inlineStr">
         <is>
           <t>(-50, 0)</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -1337,7 +1477,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>(-27.159999999999933, 0)</t>
+          <t>(-29.240000000000038, 0)</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1358,6 +1498,11 @@
       <c r="F29" t="inlineStr">
         <is>
           <t>(-50, 0)</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -1369,7 +1514,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>(-26.319999999999933, 0)</t>
+          <t>(-28.480000000000036, 0)</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1390,6 +1535,11 @@
       <c r="F30" t="inlineStr">
         <is>
           <t>(-50, 0)</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -1401,7 +1551,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>(-25.479999999999933, 0)</t>
+          <t>(-27.720000000000034, 0)</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1411,7 +1561,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>(-49.16, 0)</t>
+          <t>(-49.24, 0)</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1422,6 +1572,11 @@
       <c r="F31" t="inlineStr">
         <is>
           <t>(-50, 0)</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -1433,7 +1588,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>(-24.639999999999933, 0)</t>
+          <t>(-26.960000000000033, 0)</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1443,7 +1598,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>(-48.31999999999999, 0)</t>
+          <t>(-48.480000000000004, 0)</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1454,6 +1609,11 @@
       <c r="F32" t="inlineStr">
         <is>
           <t>(-50, 0)</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -1465,7 +1625,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>(-23.799999999999933, 0)</t>
+          <t>(-26.20000000000003, 0)</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1475,7 +1635,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>(-47.47999999999999, 0)</t>
+          <t>(-47.720000000000006, 0)</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1486,6 +1646,11 @@
       <c r="F33" t="inlineStr">
         <is>
           <t>(-50, 0)</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -1497,7 +1662,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>(-22.959999999999933, 0)</t>
+          <t>(-25.44000000000003, 0)</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1507,7 +1672,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>(-46.639999999999986, 0)</t>
+          <t>(-46.96000000000001, 0)</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1518,6 +1683,11 @@
       <c r="F34" t="inlineStr">
         <is>
           <t>(-50, 0)</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -1529,7 +1699,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>(-22.119999999999933, 0)</t>
+          <t>(-24.680000000000028, 0)</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1539,7 +1709,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>(-45.79999999999998, 0)</t>
+          <t>(-46.20000000000001, 0)</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1550,6 +1720,11 @@
       <c r="F35" t="inlineStr">
         <is>
           <t>(-50, 0)</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -1561,7 +1736,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>(-21.279999999999934, 0)</t>
+          <t>(-23.920000000000027, 0)</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1571,7 +1746,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>(-44.95999999999998, 0)</t>
+          <t>(-45.44000000000001, 0)</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1582,6 +1757,11 @@
       <c r="F36" t="inlineStr">
         <is>
           <t>(-50, 0)</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -1593,7 +1773,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>(-20.439999999999934, 0)</t>
+          <t>(-23.160000000000025, 0)</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1603,7 +1783,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>(-44.119999999999976, 0)</t>
+          <t>(-44.680000000000014, 0)</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1614,6 +1794,11 @@
       <c r="F37" t="inlineStr">
         <is>
           <t>(-50, 0)</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -1625,7 +1810,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>(-19.599999999999934, 0)</t>
+          <t>(-22.400000000000023, 0)</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1635,7 +1820,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>(-43.27999999999997, 0)</t>
+          <t>(-43.920000000000016, 0)</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -1645,7 +1830,12 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>(-49.16, 0)</t>
+          <t>(-49.24, 0)</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -1657,7 +1847,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>(-18.759999999999934, 0)</t>
+          <t>(-21.640000000000022, 0)</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1667,7 +1857,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>(-42.43999999999997, 0)</t>
+          <t>(-43.16000000000002, 0)</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -1677,7 +1867,12 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>(-48.31999999999999, 0)</t>
+          <t>(-48.480000000000004, 0)</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -1689,7 +1884,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>(-17.919999999999934, 0)</t>
+          <t>(-20.88000000000002, 0)</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1699,7 +1894,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>(-41.599999999999966, 0)</t>
+          <t>(-42.40000000000002, 0)</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -1709,7 +1904,12 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>(-47.47999999999999, 0)</t>
+          <t>(-47.720000000000006, 0)</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>(0, -50)</t>
         </is>
       </c>
     </row>
@@ -1721,7 +1921,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>(-17.079999999999934, 0)</t>
+          <t>(-20.12000000000002, 0)</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1731,7 +1931,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>(-40.75999999999996, 0)</t>
+          <t>(-41.64000000000002, 0)</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -1741,7 +1941,12 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>(-46.639999999999986, 0)</t>
+          <t>(-46.96000000000001, 0)</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>(0, -49)</t>
         </is>
       </c>
     </row>
@@ -1753,7 +1958,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>(-16.239999999999934, 0)</t>
+          <t>(-19.360000000000017, 0)</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1763,7 +1968,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>(-39.91999999999996, 0)</t>
+          <t>(-40.880000000000024, 0)</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -1773,7 +1978,12 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>(-45.79999999999998, 0)</t>
+          <t>(-46.20000000000001, 0)</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>(0, -48)</t>
         </is>
       </c>
     </row>
@@ -1785,7 +1995,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>(-15.399999999999935, 0)</t>
+          <t>(-18.600000000000016, 0)</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1795,7 +2005,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>(-39.079999999999956, 0)</t>
+          <t>(-40.120000000000026, 0)</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -1805,7 +2015,12 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>(-44.95999999999998, 0)</t>
+          <t>(-45.44000000000001, 0)</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>(0, -47)</t>
         </is>
       </c>
     </row>
@@ -1817,7 +2032,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>(-14.559999999999935, 0)</t>
+          <t>(-17.840000000000014, 0)</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1827,7 +2042,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>(-38.23999999999995, 0)</t>
+          <t>(-39.36000000000003, 0)</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -1837,7 +2052,12 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>(-44.119999999999976, 0)</t>
+          <t>(-44.680000000000014, 0)</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>(0, -46)</t>
         </is>
       </c>
     </row>
@@ -1849,7 +2069,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>(-13.719999999999935, 0)</t>
+          <t>(-17.080000000000013, 0)</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1859,7 +2079,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>(-37.39999999999995, 0)</t>
+          <t>(-38.60000000000003, 0)</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -1869,7 +2089,12 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>(-43.27999999999997, 0)</t>
+          <t>(-43.920000000000016, 0)</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>(0, -45)</t>
         </is>
       </c>
     </row>
@@ -1881,7 +2106,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>(-12.879999999999935, 0)</t>
+          <t>(-16.32000000000001, 0)</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1891,7 +2116,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>(-36.559999999999945, 0)</t>
+          <t>(-37.84000000000003, 0)</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -1901,7 +2126,12 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>(-42.43999999999997, 0)</t>
+          <t>(-43.16000000000002, 0)</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>(0, -44)</t>
         </is>
       </c>
     </row>
@@ -1913,7 +2143,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>(-12.039999999999935, 0)</t>
+          <t>(-15.560000000000011, 0)</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1923,7 +2153,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>(-35.71999999999994, 0)</t>
+          <t>(-37.080000000000034, 0)</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -1933,7 +2163,12 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>(-41.599999999999966, 0)</t>
+          <t>(-42.40000000000002, 0)</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>(0, -43)</t>
         </is>
       </c>
     </row>
@@ -1945,7 +2180,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>(-11.199999999999935, 0)</t>
+          <t>(-14.800000000000011, 0)</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1955,7 +2190,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>(-34.87999999999994, 0)</t>
+          <t>(-36.320000000000036, 0)</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -1965,7 +2200,12 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>(-40.75999999999996, 0)</t>
+          <t>(-41.64000000000002, 0)</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>(0, -42)</t>
         </is>
       </c>
     </row>
@@ -1977,7 +2217,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>(-10.359999999999935, 0)</t>
+          <t>(-14.040000000000012, 0)</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1987,7 +2227,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>(-34.039999999999935, 0)</t>
+          <t>(-35.56000000000004, 0)</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -1997,7 +2237,12 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>(-39.91999999999996, 0)</t>
+          <t>(-40.880000000000024, 0)</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>(0, -41)</t>
         </is>
       </c>
     </row>
@@ -2009,7 +2254,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>(-9.519999999999936, 0)</t>
+          <t>(-13.280000000000012, 0)</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2019,7 +2264,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>(-33.19999999999993, 0)</t>
+          <t>(-34.80000000000004, 0)</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -2029,7 +2274,12 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>(-39.079999999999956, 0)</t>
+          <t>(-40.120000000000026, 0)</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>(0, -40)</t>
         </is>
       </c>
     </row>
@@ -2041,7 +2291,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>(-8.679999999999936, 0)</t>
+          <t>(-12.520000000000012, 0)</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2051,7 +2301,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>(-32.35999999999993, 0)</t>
+          <t>(-34.04000000000004, 0)</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -2061,7 +2311,12 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>(-38.23999999999995, 0)</t>
+          <t>(-39.36000000000003, 0)</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>(0, -39)</t>
         </is>
       </c>
     </row>
@@ -2073,7 +2328,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>(-7.839999999999936, 0)</t>
+          <t>(-11.760000000000012, 0)</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2083,7 +2338,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>(-31.51999999999993, 0)</t>
+          <t>(-33.280000000000044, 0)</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -2093,19 +2348,24 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>(-37.39999999999995, 0)</t>
+          <t>(-38.60000000000003, 0)</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>(0, -38)</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>(1.8399999999999999, 0)</t>
+          <t>(1.76, 0)</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>(-6.999999999999936, 0)</t>
+          <t>(-11.000000000000012, 0)</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2115,7 +2375,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>(-30.67999999999993, 0)</t>
+          <t>(-32.520000000000046, 0)</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -2125,19 +2385,24 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>(-36.559999999999945, 0)</t>
+          <t>(-37.84000000000003, 0)</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>(0, -37)</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>(2.6799999999999997, 0)</t>
+          <t>(2.52, 0)</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>(-6.159999999999936, 0)</t>
+          <t>(-10.240000000000013, 0)</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2147,7 +2412,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>(-29.83999999999993, 0)</t>
+          <t>(-31.760000000000044, 0)</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -2157,19 +2422,24 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>(-35.71999999999994, 0)</t>
+          <t>(-37.080000000000034, 0)</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>(0, -36)</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>(3.5199999999999996, 0)</t>
+          <t>(3.2800000000000002, 0)</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>(-5.319999999999936, 0)</t>
+          <t>(-9.480000000000013, 0)</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2179,7 +2449,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>(-28.99999999999993, 0)</t>
+          <t>(-31.000000000000043, 0)</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -2189,19 +2459,24 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>(-34.87999999999994, 0)</t>
+          <t>(-36.320000000000036, 0)</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>(0, -35)</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>(4.359999999999999, 0)</t>
+          <t>(4.04, 0)</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>(-4.4799999999999365, 0)</t>
+          <t>(-8.720000000000013, 0)</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2211,7 +2486,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>(-28.15999999999993, 0)</t>
+          <t>(-30.24000000000004, 0)</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -2221,19 +2496,24 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>(-34.039999999999935, 0)</t>
+          <t>(-35.56000000000004, 0)</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>(0, -34)</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>(5.199999999999999, 0)</t>
+          <t>(4.8, 0)</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>(-3.6399999999999366, 0)</t>
+          <t>(-7.960000000000013, 0)</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2243,7 +2523,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>(-27.31999999999993, 0)</t>
+          <t>(-29.48000000000004, 0)</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -2253,19 +2533,24 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>(-33.19999999999993, 0)</t>
+          <t>(-34.80000000000004, 0)</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>(0, -33)</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>(6.039999999999999, 0)</t>
+          <t>(5.56, 0)</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>(-2.7999999999999368, 0)</t>
+          <t>(-7.2000000000000135, 0)</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2275,7 +2560,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>(-26.47999999999993, 0)</t>
+          <t>(-28.720000000000038, 0)</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -2285,19 +2570,24 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>(-32.35999999999993, 0)</t>
+          <t>(-34.04000000000004, 0)</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>(0, -32)</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>(6.879999999999999, 0)</t>
+          <t>(6.319999999999999, 0)</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>(-1.959999999999937, 0)</t>
+          <t>(-6.440000000000014, 0)</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2307,7 +2597,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>(-25.63999999999993, 0)</t>
+          <t>(-27.960000000000036, 0)</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -2317,19 +2607,24 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>(-31.51999999999993, 0)</t>
+          <t>(-33.280000000000044, 0)</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>(0, -31)</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>(7.719999999999999, 0)</t>
+          <t>(7.079999999999999, 0)</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>(-1.119999999999937, 0)</t>
+          <t>(-5.680000000000014, 0)</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2339,7 +2634,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>(-24.79999999999993, 0)</t>
+          <t>(-27.200000000000035, 0)</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -2349,19 +2644,24 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>(-30.67999999999993, 0)</t>
+          <t>(-32.520000000000046, 0)</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>(0, -30)</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>(8.559999999999999, 0)</t>
+          <t>(7.839999999999999, 0)</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>(1, -1)</t>
+          <t>(-4.920000000000014, 0)</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2371,7 +2671,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>(-23.95999999999993, 0)</t>
+          <t>(-26.440000000000033, 0)</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -2381,19 +2681,24 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>(-29.83999999999993, 0)</t>
+          <t>(-31.760000000000044, 0)</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>(0, -29)</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(8.6, 0)</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>(1, -2)</t>
+          <t>(-4.160000000000014, 0)</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2403,7 +2708,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>(-23.11999999999993, 0)</t>
+          <t>(-25.68000000000003, 0)</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
@@ -2413,19 +2718,24 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>(-28.99999999999993, 0)</t>
+          <t>(-31.000000000000043, 0)</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>(0, -28)</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>(1, -3)</t>
+          <t>(-3.4000000000000146, 0)</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2435,7 +2745,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>(-22.27999999999993, 0)</t>
+          <t>(-24.92000000000003, 0)</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
@@ -2445,19 +2755,24 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>(-28.15999999999993, 0)</t>
+          <t>(-30.24000000000004, 0)</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>(0, -27)</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>(1, -4)</t>
+          <t>(-2.640000000000015, 0)</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2467,7 +2782,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>(-21.43999999999993, 0)</t>
+          <t>(-24.16000000000003, 0)</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -2477,19 +2792,24 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>(-27.31999999999993, 0)</t>
+          <t>(-29.48000000000004, 0)</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>(0, -26)</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>(1, -5)</t>
+          <t>(-1.8800000000000148, 0)</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2499,7 +2819,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>(-20.59999999999993, 0)</t>
+          <t>(-23.400000000000027, 0)</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -2509,19 +2829,24 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>(-26.47999999999993, 0)</t>
+          <t>(-28.720000000000038, 0)</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>(0, -25)</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>(1, -6)</t>
+          <t>(-1.1200000000000148, 0)</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2531,7 +2856,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>(-19.75999999999993, 0)</t>
+          <t>(-22.640000000000025, 0)</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -2541,19 +2866,24 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>(-25.63999999999993, 0)</t>
+          <t>(-27.960000000000036, 0)</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>(0, -24)</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>(1, -7)</t>
+          <t>(1, -1)</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2563,7 +2893,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>(-18.91999999999993, 0)</t>
+          <t>(-21.880000000000024, 0)</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -2573,19 +2903,24 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>(-24.79999999999993, 0)</t>
+          <t>(-27.200000000000035, 0)</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>(0, -23)</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>(1, -8)</t>
+          <t>(1, -2)</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2595,7 +2930,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>(-18.07999999999993, 0)</t>
+          <t>(-21.120000000000022, 0)</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -2605,19 +2940,24 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>(-23.95999999999993, 0)</t>
+          <t>(-26.440000000000033, 0)</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>(0, -22)</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>(1, -9)</t>
+          <t>(1, -3)</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2627,7 +2967,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>(-17.23999999999993, 0)</t>
+          <t>(-20.36000000000002, 0)</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -2637,19 +2977,24 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>(-23.11999999999993, 0)</t>
+          <t>(-25.68000000000003, 0)</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>(0, -21)</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>(1, -9)</t>
+          <t>(1, -4)</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2659,7 +3004,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>(-16.39999999999993, 0)</t>
+          <t>(-19.60000000000002, 0)</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -2669,19 +3014,24 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>(-22.27999999999993, 0)</t>
+          <t>(-24.92000000000003, 0)</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>(0, -20)</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>(1, -9)</t>
+          <t>(1, -5)</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2691,7 +3041,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>(-15.559999999999931, 0)</t>
+          <t>(-18.840000000000018, 0)</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -2701,19 +3051,24 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>(-21.43999999999993, 0)</t>
+          <t>(-24.16000000000003, 0)</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>(0, -19)</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>(1, -9)</t>
+          <t>(1, -6)</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2723,7 +3078,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>(-14.719999999999931, 0)</t>
+          <t>(-18.080000000000016, 0)</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -2733,19 +3088,24 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>(-20.59999999999993, 0)</t>
+          <t>(-23.400000000000027, 0)</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>(0, -18)</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>(1, -9)</t>
+          <t>(1, -7)</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2755,7 +3115,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>(-13.879999999999932, 0)</t>
+          <t>(-17.320000000000014, 0)</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
@@ -2765,19 +3125,24 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>(-19.75999999999993, 0)</t>
+          <t>(-22.640000000000025, 0)</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>(0, -17)</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>(1, -9)</t>
+          <t>(1, -8)</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2787,7 +3152,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>(-13.039999999999932, 0)</t>
+          <t>(-16.560000000000013, 0)</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -2797,14 +3162,19 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>(-18.91999999999993, 0)</t>
+          <t>(-21.880000000000024, 0)</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>(0, -16)</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2819,7 +3189,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>(-12.199999999999932, 0)</t>
+          <t>(-15.800000000000013, 0)</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
@@ -2829,14 +3199,19 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>(-18.07999999999993, 0)</t>
+          <t>(-21.120000000000022, 0)</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>(0, -15)</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2851,7 +3226,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>(-11.359999999999932, 0)</t>
+          <t>(-15.040000000000013, 0)</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -2861,14 +3236,19 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>(-17.23999999999993, 0)</t>
+          <t>(-20.36000000000002, 0)</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>(0, -14)</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2883,7 +3263,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>(-10.519999999999932, 0)</t>
+          <t>(-14.280000000000014, 0)</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
@@ -2893,14 +3273,19 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>(-16.39999999999993, 0)</t>
+          <t>(-19.60000000000002, 0)</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>(0, -13)</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2910,12 +3295,12 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>(1.8399999999999999, 0)</t>
+          <t>(1.76, 0)</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>(-9.679999999999932, 0)</t>
+          <t>(-13.520000000000014, 0)</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
@@ -2925,14 +3310,19 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>(-15.559999999999931, 0)</t>
+          <t>(-18.840000000000018, 0)</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>(0, -12)</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2942,12 +3332,12 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>(2.6799999999999997, 0)</t>
+          <t>(2.52, 0)</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>(-8.839999999999932, 0)</t>
+          <t>(-12.760000000000014, 0)</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
@@ -2957,14 +3347,19 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>(-14.719999999999931, 0)</t>
+          <t>(-18.080000000000016, 0)</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>(0, -11)</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2974,12 +3369,12 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>(3.5199999999999996, 0)</t>
+          <t>(3.2800000000000002, 0)</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>(-7.9999999999999325, 0)</t>
+          <t>(-12.000000000000014, 0)</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
@@ -2989,14 +3384,19 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>(-13.879999999999932, 0)</t>
+          <t>(-17.320000000000014, 0)</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>(0, -10)</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -3006,12 +3406,12 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>(4.359999999999999, 0)</t>
+          <t>(4.04, 0)</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>(-7.159999999999933, 0)</t>
+          <t>(-11.240000000000014, 0)</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
@@ -3021,14 +3421,19 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>(-13.039999999999932, 0)</t>
+          <t>(-16.560000000000013, 0)</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>(0, -9)</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -3038,12 +3443,12 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>(5.199999999999999, 0)</t>
+          <t>(4.8, 0)</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>(-6.319999999999933, 0)</t>
+          <t>(-10.480000000000015, 0)</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
@@ -3053,14 +3458,19 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>(-12.199999999999932, 0)</t>
+          <t>(-15.800000000000013, 0)</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>(0, -8)</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -3070,12 +3480,12 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>(6.039999999999999, 0)</t>
+          <t>(5.56, 0)</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>(-5.479999999999933, 0)</t>
+          <t>(-9.720000000000015, 0)</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
@@ -3085,14 +3495,19 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>(-11.359999999999932, 0)</t>
+          <t>(-15.040000000000013, 0)</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>(0, -7)</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -3102,12 +3517,12 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>(6.879999999999999, 0)</t>
+          <t>(6.319999999999999, 0)</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>(-4.639999999999933, 0)</t>
+          <t>(-8.960000000000015, 0)</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
@@ -3117,14 +3532,19 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>(-10.519999999999932, 0)</t>
+          <t>(-14.280000000000014, 0)</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>(0, -6)</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -3134,29 +3554,34 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>(7.719999999999999, 0)</t>
+          <t>(7.079999999999999, 0)</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>(-3.799999999999933, 0)</t>
+          <t>(-8.200000000000015, 0)</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>(1.8399999999999999, 0)</t>
+          <t>(1.76, 0)</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>(-9.679999999999932, 0)</t>
+          <t>(-13.520000000000014, 0)</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>(0, -5)</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -3166,29 +3591,34 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>(8.559999999999999, 0)</t>
+          <t>(7.839999999999999, 0)</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>(-2.9599999999999334, 0)</t>
+          <t>(-7.4400000000000155, 0)</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>(2.6799999999999997, 0)</t>
+          <t>(2.52, 0)</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>(-8.839999999999932, 0)</t>
+          <t>(-12.760000000000014, 0)</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>(0, -4)</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -3198,29 +3628,34 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(8.6, 0)</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>(-2.1199999999999335, 0)</t>
+          <t>(-6.680000000000016, 0)</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>(3.5199999999999996, 0)</t>
+          <t>(3.2800000000000002, 0)</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>(-7.9999999999999325, 0)</t>
+          <t>(-12.000000000000014, 0)</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>(0, -3)</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -3230,29 +3665,34 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>(-1.2799999999999336, 0)</t>
+          <t>(-5.920000000000016, 0)</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>(4.359999999999999, 0)</t>
+          <t>(4.04, 0)</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>(-7.159999999999933, 0)</t>
+          <t>(-11.240000000000014, 0)</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>(0, -2)</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -3262,29 +3702,34 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>(1, -1)</t>
+          <t>(-5.160000000000016, 0)</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>(5.199999999999999, 0)</t>
+          <t>(4.8, 0)</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>(-6.319999999999933, 0)</t>
+          <t>(-10.480000000000015, 0)</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>(0, -1)</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -3294,29 +3739,34 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>(1, -2)</t>
+          <t>(-4.400000000000016, 0)</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>(6.039999999999999, 0)</t>
+          <t>(5.56, 0)</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>(-5.479999999999933, 0)</t>
+          <t>(-9.720000000000015, 0)</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>(1, 0)</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -3326,29 +3776,34 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>(1, -3)</t>
+          <t>(-3.6400000000000166, 0)</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>(6.879999999999999, 0)</t>
+          <t>(6.319999999999999, 0)</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>(-4.639999999999933, 0)</t>
+          <t>(-8.960000000000015, 0)</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>(1.76, 0)</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -3358,29 +3813,34 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>(1, -4)</t>
+          <t>(-2.8800000000000168, 0)</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>(7.719999999999999, 0)</t>
+          <t>(7.079999999999999, 0)</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>(-3.799999999999933, 0)</t>
+          <t>(-8.200000000000015, 0)</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>(2.52, 0)</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -3390,29 +3850,34 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>(1, -5)</t>
+          <t>(-2.120000000000017, 0)</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>(8.559999999999999, 0)</t>
+          <t>(7.839999999999999, 0)</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>(-2.9599999999999334, 0)</t>
+          <t>(-7.4400000000000155, 0)</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>(3.2800000000000002, 0)</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -3422,29 +3887,34 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>(1, -6)</t>
+          <t>(-1.360000000000017, 0)</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(8.6, 0)</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>(-2.1199999999999335, 0)</t>
+          <t>(-6.680000000000016, 0)</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>(4.04, 0)</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -3454,29 +3924,34 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>(1, -7)</t>
+          <t>(1, -1)</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>(-1.2799999999999336, 0)</t>
+          <t>(-5.920000000000016, 0)</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>(4.8, 0)</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -3486,29 +3961,34 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>(1, -8)</t>
+          <t>(1, -2)</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>(1, -1)</t>
+          <t>(-5.160000000000016, 0)</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>(5.56, 0)</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -3518,29 +3998,34 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>(1, -9)</t>
+          <t>(1, -3)</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>(1, -2)</t>
+          <t>(-4.400000000000016, 0)</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>(6.319999999999999, 0)</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -3550,29 +4035,34 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>(1, -9)</t>
+          <t>(1, -4)</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>(1, -3)</t>
+          <t>(-3.6400000000000166, 0)</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>(7.079999999999999, 0)</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -3582,29 +4072,34 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>(1, -9)</t>
+          <t>(1, -5)</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>(1, -4)</t>
+          <t>(-2.8800000000000168, 0)</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>(7.839999999999999, 0)</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -3614,29 +4109,34 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>(1, -9)</t>
+          <t>(1, -6)</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>(1, -5)</t>
+          <t>(-2.120000000000017, 0)</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>(8.6, 0)</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -3646,29 +4146,34 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>(1, -9)</t>
+          <t>(1, -7)</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>(1, -6)</t>
+          <t>(-1.360000000000017, 0)</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>(9.36, 0)</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -3678,29 +4183,34 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>(1, -9)</t>
+          <t>(1, -8)</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>(1, -7)</t>
+          <t>(1, -1)</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>(9.36, 0)</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -3710,7 +4220,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -3720,19 +4230,24 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>(1, -8)</t>
+          <t>(1, -2)</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>(9.36, 0)</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -3742,7 +4257,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -3752,12 +4267,239 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>(9.399999999999999, 0)</t>
+          <t>(9.36, 0)</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
         <is>
+          <t>(1, -3)</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>(9.36, 0)</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>(9.36, 0)</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
           <t>(1, -9)</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>(9.36, 0)</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>(1, -9)</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>(9.36, 0)</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>(1, -4)</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>(9.36, 0)</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>(9.36, 0)</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>(1, -9)</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>(9.36, 0)</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>(1, -9)</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>(9.36, 0)</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>(1, -5)</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>(9.36, 0)</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>(9.36, 0)</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>(1, -9)</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>(9.36, 0)</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>(1, -9)</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>(9.36, 0)</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>(1, -6)</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>(9.36, 0)</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>(9.36, 0)</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>(1, -9)</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>(9.36, 0)</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>(1, -9)</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>(9.36, 0)</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>(1, -7)</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>(9.36, 0)</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>(9.36, 0)</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>(1, -9)</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>(9.36, 0)</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>(1, -9)</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>(9.36, 0)</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>(1, -8)</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>(9.36, 0)</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>(9.36, 0)</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>(1, -9)</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>(9.36, 0)</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>(1, -9)</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>(9.36, 0)</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>(1, -9)</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>(9.36, 0)</t>
         </is>
       </c>
     </row>

</xml_diff>